<commit_message>
Add the two files
max signup and login
</commit_message>
<xml_diff>
--- a/testcases/usernames.xlsx
+++ b/testcases/usernames.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\QAT_SRDS\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEE5CD05-8BDB-4F42-8BEF-9EDDAB72B351}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47425828-FB34-4091-9AA4-8E3CDDA305A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{596A4F95-E419-4015-869E-B8B8569DA6F4}"/>
   </bookViews>
@@ -25,18 +25,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>user_name</t>
   </si>
   <si>
-    <t>omkarhundre+201@arcitech.ai</t>
-  </si>
-  <si>
     <t>Testcase_no.</t>
   </si>
   <si>
-    <t>omkarhundre+202@arcitech.ai</t>
+    <t>omkarhundre+215@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+216@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+217@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+218@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+219@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+220@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+221@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+222@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+223@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+224@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+225@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+226@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+227@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+228@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+229@arcitech.ai</t>
+  </si>
+  <si>
+    <t>omkarhundre+230@arcitech.ai</t>
   </si>
 </sst>
 </file>
@@ -408,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB1E37D-2C62-4088-858A-9D552ECD05EB}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -422,7 +464,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -433,7 +475,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -444,12 +486,148 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{D9AD85CC-E258-4CF9-A2D3-4F7EF9259C30}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{43C809B7-2B34-4923-8759-420EEFA7C00C}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{6AB7E02D-696C-413C-A874-1C18562552A1}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{0677FA36-DC33-4CCE-AFE1-87C0CF18967C}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{74739E52-11F6-4FFB-92E9-567BC778ACCB}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{EE795704-4C9E-4404-BD19-83D436D5DA4C}"/>
+    <hyperlink ref="B6" r:id="rId5" xr:uid="{E777E5F7-D3F9-405D-B932-4D52F75C0D5A}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{EC84259D-FD05-4A93-A598-F2D83F1736CA}"/>
+    <hyperlink ref="B8" r:id="rId7" xr:uid="{FC023779-E516-4928-91D6-4AF345D2C23F}"/>
+    <hyperlink ref="B9" r:id="rId8" xr:uid="{91E88581-4485-451E-9F23-EEB84D705A83}"/>
+    <hyperlink ref="B10" r:id="rId9" xr:uid="{2C463D15-1492-4526-8DC5-6E06DDD68FF2}"/>
+    <hyperlink ref="B11" r:id="rId10" xr:uid="{FE410104-914D-48E5-A88C-16906BDB7DEF}"/>
+    <hyperlink ref="B12" r:id="rId11" xr:uid="{999F1EB6-D729-4A36-8E97-E266B42C3D37}"/>
+    <hyperlink ref="B13" r:id="rId12" xr:uid="{0EA468C8-2B81-48E4-BFAA-163F7CC31244}"/>
+    <hyperlink ref="B14" r:id="rId13" xr:uid="{47136FB4-03CB-4F92-B9F0-5E45A5556478}"/>
+    <hyperlink ref="B15" r:id="rId14" xr:uid="{DA279C42-5D16-4BC0-91E7-7BDD3C736DAC}"/>
+    <hyperlink ref="B16" r:id="rId15" xr:uid="{3CDFFEB0-C9F5-4014-9DEA-31AFC716C022}"/>
+    <hyperlink ref="B17" r:id="rId16" xr:uid="{2E9BFE01-7EB9-4E23-A235-ABAC69221B4C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>